<commit_message>
Changed up the counties.
</commit_message>
<xml_diff>
--- a/north-virginia-2024.xlsx
+++ b/north-virginia-2024.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -593,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,7 +720,7 @@
         <v>54021</v>
       </c>
       <c r="C11">
-        <v>56.4</v>
+        <v>-57.9</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -731,7 +731,7 @@
         <v>54023</v>
       </c>
       <c r="C12">
-        <v>-76.400000000000006</v>
+        <v>-68.2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -819,7 +819,7 @@
         <v>54041</v>
       </c>
       <c r="C20">
-        <v>-64.400000000000006</v>
+        <v>-57.8</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -863,7 +863,7 @@
         <v>54049</v>
       </c>
       <c r="C24">
-        <v>58.8</v>
+        <v>-54.9</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -951,7 +951,7 @@
         <v>54067</v>
       </c>
       <c r="C32">
-        <v>-56.5</v>
+        <v>54.8</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -984,7 +984,7 @@
         <v>54075</v>
       </c>
       <c r="C35">
-        <v>-53.5</v>
+        <v>54.7</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1083,7 +1083,7 @@
         <v>54093</v>
       </c>
       <c r="C44">
-        <v>-64.400000000000006</v>
+        <v>-57.9</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1127,7 +1127,7 @@
         <v>54101</v>
       </c>
       <c r="C48">
-        <v>-56.9</v>
+        <v>52.7</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1160,7 +1160,7 @@
         <v>54107</v>
       </c>
       <c r="C51">
-        <v>-65.099999999999994</v>
+        <v>-53.7</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1193,7 +1193,7 @@
         <v>24001</v>
       </c>
       <c r="C54">
-        <v>-67.8</v>
+        <v>-74.3</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cleaned up the file names and some code for the cities.
</commit_message>
<xml_diff>
--- a/north-virginia-2024.xlsx
+++ b/north-virginia-2024.xlsx
@@ -594,7 +594,7 @@
   <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V17" sqref="V17"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,7 +632,7 @@
         <v>54003</v>
       </c>
       <c r="C3">
-        <v>-56.4</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -731,7 +731,7 @@
         <v>54023</v>
       </c>
       <c r="C12">
-        <v>-68.2</v>
+        <v>-56.4</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1182,7 +1182,7 @@
         <v>24023</v>
       </c>
       <c r="C53">
-        <v>-64.599999999999994</v>
+        <v>-57.4</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed a broken county.
</commit_message>
<xml_diff>
--- a/north-virginia-2024.xlsx
+++ b/north-virginia-2024.xlsx
@@ -594,7 +594,7 @@
   <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,7 +632,7 @@
         <v>54003</v>
       </c>
       <c r="C3">
-        <v>51</v>
+        <v>-64.599999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>